<commit_message>
update anh Tuan NB
</commit_message>
<xml_diff>
--- a/4.Workspace/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2025/Thang1/02.TraBH/TBH_AnhTuanNB_080125.xlsx
+++ b/4.Workspace/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2025/Thang1/02.TraBH/TBH_AnhTuanNB_080125.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$28</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t xml:space="preserve">STT </t>
   </si>
@@ -141,6 +141,51 @@
   <si>
     <t>ID mới: 
 WM21051100S0167 / 00BD00079</t>
+  </si>
+  <si>
+    <t>ID mới: 202412316688033</t>
+  </si>
+  <si>
+    <t>ID mới: 202412316688046</t>
+  </si>
+  <si>
+    <t>ID mới: 202412316688026</t>
+  </si>
+  <si>
+    <t>ID mới: 202412316688028</t>
+  </si>
+  <si>
+    <t>VNSH02</t>
+  </si>
+  <si>
+    <t>WP21110069S00686 / 00320013EA</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>WP21110052S00610 / 0032001014</t>
+  </si>
+  <si>
+    <t>Thiết bị thường xuyên mất GPS</t>
+  </si>
+  <si>
+    <t>WP21110069S00984 / 00320014A9</t>
+  </si>
+  <si>
+    <t>WP21110069S00976 / 0032001255</t>
+  </si>
+  <si>
+    <t>Camera cabin bị nhiễu trắng</t>
+  </si>
+  <si>
+    <t>0032007B92</t>
+  </si>
+  <si>
+    <t>WP21110052S00936 / 003200123D</t>
+  </si>
+  <si>
+    <t>Đổi thiết bị khác, phí sửa chữa thiết bị cũ VNET phản hồi lại khách hàng sau</t>
   </si>
 </sst>
 </file>
@@ -270,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -513,6 +558,30 @@
       <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -523,7 +592,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -599,6 +668,43 @@
     <xf numFmtId="3" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -703,10 +809,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1065,10 +1167,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="85" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:I7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="130" zoomScaleNormal="85" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1180,7 @@
     <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="24.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="14" style="4" customWidth="1"/>
@@ -1088,124 +1190,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="56" t="s">
+      <c r="A1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="58"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="71"/>
     </row>
     <row r="2" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="59" t="s">
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="62" t="s">
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="77"/>
     </row>
     <row r="4" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="65" t="s">
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="67"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="80"/>
     </row>
     <row r="5" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="59"/>
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
     </row>
     <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
       <c r="M8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="55"/>
       <c r="L9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1244,21 +1346,23 @@
       <c r="A11" s="28">
         <v>1</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="69">
+      <c r="C11" s="35">
         <v>170420240005</v>
       </c>
       <c r="D11" s="27"/>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27" t="s">
+      <c r="F11" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="43" t="s">
         <v>36</v>
       </c>
       <c r="I11" s="29"/>
@@ -1268,23 +1372,19 @@
       <c r="A12" s="28">
         <v>2</v>
       </c>
-      <c r="B12" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="69">
+      <c r="B12" s="41"/>
+      <c r="C12" s="35">
         <v>202410050835019</v>
       </c>
       <c r="D12" s="27"/>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>36</v>
-      </c>
+      <c r="F12" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
       <c r="I12" s="29"/>
       <c r="J12" s="7"/>
     </row>
@@ -1292,23 +1392,19 @@
       <c r="A13" s="28">
         <v>3</v>
       </c>
-      <c r="B13" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="69">
+      <c r="B13" s="41"/>
+      <c r="C13" s="35">
         <v>202410050835020</v>
       </c>
       <c r="D13" s="27"/>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>36</v>
-      </c>
+      <c r="F13" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="29"/>
       <c r="J13" s="7"/>
     </row>
@@ -1316,48 +1412,44 @@
       <c r="A14" s="28">
         <v>4</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="69">
+      <c r="B14" s="42"/>
+      <c r="C14" s="35">
         <v>202410050835009</v>
       </c>
       <c r="D14" s="27"/>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>36</v>
-      </c>
+      <c r="F14" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="29"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28">
         <v>5</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>27</v>
+      <c r="B15" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>44</v>
       </c>
       <c r="D15" s="27"/>
-      <c r="E15" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>32</v>
+      <c r="E15" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="43" t="s">
+        <v>53</v>
       </c>
       <c r="I15" s="29"/>
       <c r="J15" s="7"/>
@@ -1366,145 +1458,211 @@
       <c r="A16" s="28">
         <v>6</v>
       </c>
-      <c r="B16" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>29</v>
+      <c r="B16" s="41"/>
+      <c r="C16" s="35" t="s">
+        <v>48</v>
       </c>
       <c r="D16" s="27"/>
-      <c r="E16" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>32</v>
-      </c>
+      <c r="E16" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="44"/>
       <c r="I16" s="29"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+    <row r="17" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28">
+        <v>7</v>
+      </c>
+      <c r="B17" s="42"/>
+      <c r="C17" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="29"/>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17" t="s">
+    <row r="18" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28">
+        <v>8</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="29"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
+        <v>9</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="45"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="33" t="s">
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+    </row>
+    <row r="22" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="36" t="s">
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-    </row>
-    <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="9"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
     </row>
     <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="24"/>
+    </row>
+    <row r="27" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="35" t="s">
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-    </row>
-    <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="26"/>
-    </row>
-    <row r="27" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-    </row>
-    <row r="66" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+    </row>
+    <row r="28" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="26"/>
+    </row>
+    <row r="30" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+    </row>
+    <row r="69" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="23">
     <mergeCell ref="A1:C4"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="D2:I2"/>
@@ -1515,15 +1673,22 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="B6:I6"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
   </mergeCells>
-  <pageMargins left="0.5" right="1" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="86" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.5" right="1" top="0.5" bottom="0.5" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="83" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>